<commit_message>
Template change for ERM-18
</commit_message>
<xml_diff>
--- a/UserManagement/wwwroot/Template.xlsx
+++ b/UserManagement/wwwroot/Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="142">
   <si>
     <r>
       <rPr>
@@ -144,7 +144,7 @@
     <t>Assign PHC Or Hub</t>
   </si>
   <si>
-    <t>Sub Menu Id</t>
+    <t>Sub Menu</t>
   </si>
   <si>
     <t>PHC Deepika</t>
@@ -159,7 +159,7 @@
     <t>2534378589</t>
   </si>
   <si>
-    <t xml:space="preserve">  deepeka@gmail.com</t>
+    <t>deepeka@gmail.com</t>
   </si>
   <si>
     <t>PUNJAB</t>
@@ -174,13 +174,13 @@
     <t>497449</t>
   </si>
   <si>
-    <t>Ram</t>
+    <t>Sonu</t>
   </si>
   <si>
     <t>Singh</t>
   </si>
   <si>
-    <t>9942368412</t>
+    <t>9984552412</t>
   </si>
   <si>
     <t>Male</t>
@@ -192,7 +192,7 @@
     <t>1.7</t>
   </si>
   <si>
-    <t>Ram.singh253@gmail.com</t>
+    <t>Sonu.singh18@gmail.com</t>
   </si>
   <si>
     <t>19-12-1981</t>
@@ -225,7 +225,7 @@
     <t>PHC Pondibachra</t>
   </si>
   <si>
-    <t>9;8;6</t>
+    <t>Patient List,Add Patient</t>
   </si>
   <si>
     <t>PHC Advani</t>
@@ -249,22 +249,22 @@
     <t>497331</t>
   </si>
   <si>
-    <t>Kapil</t>
+    <t>Kedar</t>
   </si>
   <si>
     <t>Paswan</t>
   </si>
   <si>
-    <t>9938443845</t>
-  </si>
-  <si>
-    <t>Kapil.Paswan481@gmail.com</t>
+    <t>9934529545</t>
+  </si>
+  <si>
+    <t>Kedar.Paswn41841@gmail.com</t>
   </si>
   <si>
     <t>20-08-1982</t>
   </si>
   <si>
-    <t>5;6</t>
+    <t>User Dashboard,Cases Received</t>
   </si>
   <si>
     <t>SC Janavi Jha</t>
@@ -291,13 +291,13 @@
     <t>497339</t>
   </si>
   <si>
-    <t>Lalita</t>
+    <t>Kusum</t>
   </si>
   <si>
     <t>Paikra</t>
   </si>
   <si>
-    <t>9922354662</t>
+    <t>9235415662</t>
   </si>
   <si>
     <t>Female</t>
@@ -306,7 +306,7 @@
     <t>1.5</t>
   </si>
   <si>
-    <t>Lalita.paikra512@gmail.com</t>
+    <t>Kusum.paikr5412@gmail.com</t>
   </si>
   <si>
     <t>CHO</t>
@@ -318,7 +318,7 @@
     <t>Ms</t>
   </si>
   <si>
-    <t>5;6;7</t>
+    <t>Cases Referred</t>
   </si>
   <si>
     <t>SC Amit Dettole</t>
@@ -327,13 +327,16 @@
     <t>Amit12@gmail.com</t>
   </si>
   <si>
-    <t>9933034715</t>
-  </si>
-  <si>
-    <t>Lalita.paikra418@gmail.com</t>
-  </si>
-  <si>
-    <t>7;9</t>
+    <t>Suman</t>
+  </si>
+  <si>
+    <t>9934104715</t>
+  </si>
+  <si>
+    <t>Suman.pakra4418@gmail.com</t>
+  </si>
+  <si>
+    <t>Health Cube</t>
   </si>
   <si>
     <t>SC Simran Singh</t>
@@ -354,19 +357,19 @@
     <t>SC Amadand Korea</t>
   </si>
   <si>
-    <t>Lotus</t>
-  </si>
-  <si>
-    <t>9933224699</t>
-  </si>
-  <si>
-    <t>Lotus.paikra918@gmail.com</t>
+    <t>Lilly</t>
+  </si>
+  <si>
+    <t>9933784699</t>
+  </si>
+  <si>
+    <t>Lilly.paikra9418@gmail.com</t>
   </si>
   <si>
     <t>12-05-1984</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Cases Received,Cases Referred</t>
   </si>
   <si>
     <t>Phc Kapil Ghartonde</t>
@@ -378,16 +381,19 @@
     <t>PHC Sharma FAZILKA</t>
   </si>
   <si>
-    <t>Rose</t>
+    <t>Prisha</t>
   </si>
   <si>
     <t>Merry</t>
   </si>
   <si>
-    <t>9926214812</t>
-  </si>
-  <si>
-    <t>Rose.Merry819@gmail.com</t>
+    <t>9926634812</t>
+  </si>
+  <si>
+    <t>Prisha.Mery819@gmail.com</t>
+  </si>
+  <si>
+    <t>User Dashboard</t>
   </si>
   <si>
     <t>Hub Yash Choudhari</t>
@@ -417,19 +423,19 @@
     <t>497335</t>
   </si>
   <si>
-    <t>Brijnandan</t>
+    <t>Angela</t>
   </si>
   <si>
     <t>Sharma</t>
   </si>
   <si>
-    <t>7885974954</t>
+    <t>7886524954</t>
   </si>
   <si>
     <t>1.6</t>
   </si>
   <si>
-    <t>brijnandan.sharma215@gmail.com</t>
+    <t>Angela.shrma215@gmail.com</t>
   </si>
   <si>
     <t>02-03-1985</t>
@@ -438,7 +444,7 @@
     <t>Pune</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Patient List</t>
   </si>
   <si>
     <t>Hub Mansi kate</t>
@@ -450,13 +456,13 @@
     <t>Mansi121@gmail.com</t>
   </si>
   <si>
-    <t>7925297564</t>
-  </si>
-  <si>
-    <t>brijnandan.shar100@gmail.com</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>Fatimah</t>
+  </si>
+  <si>
+    <t>7925537564</t>
+  </si>
+  <si>
+    <t>Fatimah.shar100@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -624,6 +630,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center"/>
@@ -885,7 +894,8 @@
     <col customWidth="1" min="29" max="29" width="9.75"/>
     <col customWidth="1" min="30" max="30" width="8.5"/>
     <col customWidth="1" min="31" max="31" width="3.88"/>
-    <col customWidth="1" min="33" max="34" width="19.75"/>
+    <col customWidth="1" min="33" max="33" width="19.75"/>
+    <col customWidth="1" min="34" max="34" width="31.38"/>
   </cols>
   <sheetData>
     <row r="1" ht="45.0" customHeight="1">
@@ -1028,808 +1038,808 @@
       <c r="AG2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="13" t="s">
+      <c r="AH2" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="15">
+      <c r="A3" s="16">
         <v>1.0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="17" t="s">
+      <c r="R3" s="17"/>
+      <c r="S3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="V3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="Z3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AA3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC3" s="20" t="s">
+      <c r="AC3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="20" t="s">
+      <c r="AD3" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE3" s="20" t="s">
+      <c r="AE3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="16" t="s">
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH3" s="17" t="s">
+      <c r="AH3" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="16">
         <v>2.0</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="Q4" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16" t="s">
+      <c r="R4" s="17"/>
+      <c r="S4" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="T4" s="16" t="s">
+      <c r="T4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="U4" s="18" t="s">
+      <c r="U4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="V4" s="19" t="s">
+      <c r="V4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="16" t="s">
+      <c r="W4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X4" s="16" t="s">
+      <c r="X4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="Y4" s="16" t="s">
+      <c r="Y4" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="Z4" s="16" t="s">
+      <c r="Z4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="AA4" s="16" t="s">
+      <c r="AA4" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AB4" s="16" t="s">
+      <c r="AB4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AC4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD4" s="20" t="s">
+      <c r="AD4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE4" s="20" t="s">
+      <c r="AE4" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF4" s="21"/>
-      <c r="AG4" s="16" t="s">
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH4" s="17" t="s">
+      <c r="AH4" s="18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="16">
         <v>3.0</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="Q5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16" t="s">
+      <c r="R5" s="17"/>
+      <c r="S5" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="W5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X5" s="16" t="s">
+      <c r="X5" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Y5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Z5" s="16" t="s">
+      <c r="Z5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AA5" s="16" t="s">
+      <c r="AA5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AB5" s="16" t="s">
+      <c r="AB5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC5" s="20" t="s">
+      <c r="AC5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD5" s="20" t="s">
+      <c r="AD5" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE5" s="20" t="s">
+      <c r="AE5" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="16" t="s">
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH5" s="17" t="s">
+      <c r="AH5" s="18" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="15">
+      <c r="A6" s="16">
         <v>4.0</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="16" t="s">
+      <c r="L6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="N6" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="O6" s="16" t="s">
+      <c r="N6" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="O6" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="Q6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="T6" s="16" t="s">
+      <c r="R6" s="17"/>
+      <c r="S6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="T6" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="U6" s="18" t="s">
+      <c r="U6" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="V6" s="19" t="s">
+      <c r="V6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W6" s="16" t="s">
+      <c r="W6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X6" s="16" t="s">
+      <c r="X6" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Y6" s="16" t="s">
+      <c r="Y6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Z6" s="16" t="s">
+      <c r="Z6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AA6" s="16" t="s">
+      <c r="AA6" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AB6" s="16" t="s">
+      <c r="AB6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC6" s="20" t="s">
+      <c r="AC6" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" s="20" t="s">
+      <c r="AD6" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="16" t="s">
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH6" s="17" t="s">
-        <v>98</v>
+      <c r="AH6" s="18" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="15">
+      <c r="A7" s="16">
         <v>5.0</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="F7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="M7" s="16" t="s">
+      <c r="L7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="16" t="s">
+      <c r="N7" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="O7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="T7" s="16" t="s">
+      <c r="R7" s="17"/>
+      <c r="S7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="U7" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="V7" s="19" t="s">
+      <c r="U7" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="V7" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="W7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X7" s="16" t="s">
+      <c r="X7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Z7" s="16" t="s">
+      <c r="Z7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AA7" s="16" t="s">
+      <c r="AA7" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AB7" s="16" t="s">
+      <c r="AB7" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC7" s="20" t="s">
+      <c r="AC7" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD7" s="20" t="s">
+      <c r="AD7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE7" s="20" t="s">
+      <c r="AE7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="16" t="s">
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH7" s="16" t="s">
-        <v>109</v>
+      <c r="AH7" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="15">
+      <c r="A8" s="16">
         <v>6.0</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="B8" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="M8" s="16" t="s">
+      <c r="L8" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="M8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="N8" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="O8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" s="16" t="s">
+      <c r="Q8" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="T8" s="16" t="s">
+      <c r="R8" s="17"/>
+      <c r="S8" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="T8" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="U8" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="V8" s="19" t="s">
+      <c r="U8" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="V8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="W8" s="16" t="s">
+      <c r="W8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X8" s="16" t="s">
+      <c r="X8" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="Z8" s="16" t="s">
+      <c r="Z8" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AA8" s="16" t="s">
+      <c r="AA8" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AB8" s="16" t="s">
+      <c r="AB8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="20" t="s">
+      <c r="AC8" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD8" s="20" t="s">
+      <c r="AD8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE8" s="20" t="s">
+      <c r="AE8" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="16" t="s">
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH8" s="17" t="s">
-        <v>75</v>
+      <c r="AH8" s="18" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="15">
+      <c r="A9" s="16">
         <v>7.0</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="16" t="s">
+      <c r="F9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="G9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="H9" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="J9" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="K9" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="L9" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="M9" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="O9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="T9" s="16" t="s">
+      <c r="Q9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="R9" s="17"/>
+      <c r="S9" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="T9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="U9" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="V9" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="W9" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="X9" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y9" s="16" t="s">
+      <c r="U9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="V9" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="Z9" s="16" t="s">
+      <c r="W9" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="X9" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="AA9" s="16" t="s">
+      <c r="Y9" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z9" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AB9" s="16" t="s">
+      <c r="AB9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC9" s="20" t="s">
+      <c r="AC9" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD9" s="20" t="s">
+      <c r="AD9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE9" s="20" t="s">
+      <c r="AE9" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="16" t="s">
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH9" s="16" t="s">
-        <v>133</v>
+      <c r="AH9" s="18" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="15">
+      <c r="A10" s="16">
         <v>8.0</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="R10" s="17"/>
+      <c r="S10" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="U10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="V10" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="W10" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K10" s="16" t="s">
+      <c r="X10" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="Y10" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="Z10" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="R10" s="16"/>
-      <c r="S10" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="U10" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="V10" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="W10" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="X10" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y10" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA10" s="16" t="s">
+      <c r="AA10" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AB10" s="16" t="s">
+      <c r="AB10" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AC10" s="20" t="s">
+      <c r="AC10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD10" s="20" t="s">
+      <c r="AD10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE10" s="20" t="s">
+      <c r="AE10" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="16" t="s">
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AH10" s="16" t="s">
-        <v>139</v>
+      <c r="AH10" s="18" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>